<commit_message>
modificada planificacion e la propuesta se termino
</commit_message>
<xml_diff>
--- a/planificacion/planificacion subir.xlsx
+++ b/planificacion/planificacion subir.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6DA6D5-4E1E-4FF2-9FC1-936EA19CB2AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AC6A8B-E597-4725-BD15-6FD85B816D6B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version actual" sheetId="5" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>Revision de arquitectura lógica</t>
   </si>
   <si>
-    <t>Revisión de diagrama de clases</t>
-  </si>
-  <si>
     <t>Corrección y refactorización de codigo</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>Refinamiento de requisitos</t>
+  </si>
+  <si>
+    <t>Revisión y adaptación de diagrama de clases</t>
   </si>
 </sst>
 </file>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893B0263-59F4-40E5-9460-E43E9955B4EB}">
   <dimension ref="A1:BC107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="BA94" sqref="BA94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,7 +1239,7 @@
         <v>43983</v>
       </c>
       <c r="AV2" s="15">
-        <v>37012</v>
+        <v>43990</v>
       </c>
       <c r="AW2" s="15">
         <v>43997</v>
@@ -2221,7 +2221,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="J19" s="19"/>
       <c r="K19" s="19"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -2271,7 +2271,7 @@
     <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2280,7 +2280,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="19"/>
       <c r="K20" s="19"/>
       <c r="L20" s="1"/>
       <c r="M20" s="4"/>
@@ -2445,7 +2445,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2455,7 +2455,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="K23" s="19"/>
       <c r="L23" s="19"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -2504,7 +2504,7 @@
     <row r="24" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2514,7 +2514,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="19"/>
       <c r="L24" s="19"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -2969,7 +2969,7 @@
     <row r="32" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -3318,7 +3318,7 @@
     <row r="38" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -3492,7 +3492,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -3782,7 +3782,7 @@
         <v>28</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3841,7 +3841,7 @@
     <row r="47" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -4127,7 +4127,7 @@
     </row>
     <row r="52" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -4248,7 +4248,7 @@
     <row r="54" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -4600,7 +4600,7 @@
     <row r="60" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -4775,7 +4775,7 @@
         <v>27</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
@@ -5123,7 +5123,7 @@
         <v>28</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -5182,7 +5182,7 @@
     <row r="70" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
@@ -5355,7 +5355,7 @@
     </row>
     <row r="73" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
@@ -5476,7 +5476,7 @@
     <row r="75" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -5828,7 +5828,7 @@
     <row r="81" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -5887,7 +5887,7 @@
     <row r="82" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
@@ -6005,7 +6005,7 @@
         <v>27</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
@@ -6300,7 +6300,7 @@
     <row r="89" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -6475,7 +6475,7 @@
         <v>28</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
@@ -6534,7 +6534,7 @@
     <row r="93" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
@@ -6593,7 +6593,7 @@
     <row r="94" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
@@ -6640,11 +6640,11 @@
       <c r="AS94" s="4"/>
       <c r="AT94" s="4"/>
       <c r="AU94" s="4"/>
-      <c r="AV94" s="4"/>
-      <c r="AW94" s="4"/>
-      <c r="AX94" s="4"/>
-      <c r="AY94" s="4"/>
-      <c r="AZ94" s="4"/>
+      <c r="AV94" s="19"/>
+      <c r="AW94" s="19"/>
+      <c r="AX94" s="19"/>
+      <c r="AY94" s="19"/>
+      <c r="AZ94" s="19"/>
       <c r="BA94" s="4"/>
       <c r="BB94" s="4"/>
       <c r="BC94" s="4"/>
@@ -6825,22 +6825,22 @@
     <row r="98" spans="1:55" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="103" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="105" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="106" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A106" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="107" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A107" s="41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>